<commit_message>
added flexibility to use old method and to take edf
</commit_message>
<xml_diff>
--- a/clinical_info/Stim info.xlsx
+++ b/clinical_info/Stim info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="263">
   <si>
     <t>Ieeg name</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>3 mA</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
   <si>
     <t>HUP216_CCEP</t>
@@ -2734,8 +2737,8 @@
       <c r="C2" s="1">
         <v>170.95</v>
       </c>
-      <c r="D2" s="1">
-        <v>9347.8</v>
+      <c r="D2" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="E2" s="1">
         <v>170.95</v>
@@ -2858,7 +2861,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B2" s="1">
         <v>3.0</v>
@@ -2870,22 +2873,22 @@
         <v>30135.61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>116</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>62</v>
@@ -2893,13 +2896,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C3" s="1">
         <v>285058.36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>119</v>
@@ -2913,7 +2916,7 @@
     </row>
     <row r="4">
       <c r="F4" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>124</v>
@@ -2927,7 +2930,7 @@
     </row>
     <row r="5">
       <c r="F5" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>126</v>
@@ -2947,7 +2950,7 @@
         <v>130</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>65</v>
@@ -2955,7 +2958,7 @@
     </row>
     <row r="7">
       <c r="F7" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>52</v>
@@ -2969,7 +2972,7 @@
     </row>
     <row r="8">
       <c r="F8" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>56</v>
@@ -2983,7 +2986,7 @@
     </row>
     <row r="9">
       <c r="F9" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>26</v>
@@ -3003,7 +3006,7 @@
         <v>20</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>171</v>
@@ -3011,13 +3014,13 @@
     </row>
     <row r="11">
       <c r="F11" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>66</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>174</v>
@@ -3025,13 +3028,13 @@
     </row>
     <row r="12">
       <c r="F12" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>69</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>178</v>
@@ -3045,7 +3048,7 @@
         <v>71</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>131</v>
@@ -3059,7 +3062,7 @@
         <v>167</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>134</v>
@@ -3073,7 +3076,7 @@
         <v>169</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>175</v>
@@ -3081,13 +3084,13 @@
     </row>
     <row r="16">
       <c r="F16" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>177</v>
@@ -3095,13 +3098,13 @@
     </row>
     <row r="17">
       <c r="F17" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>179</v>
@@ -3109,13 +3112,13 @@
     </row>
     <row r="18">
       <c r="F18" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>181</v>
@@ -3123,7 +3126,7 @@
     </row>
     <row r="19">
       <c r="F19" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>59</v>
@@ -3131,7 +3134,7 @@
     </row>
     <row r="20">
       <c r="F20" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>54</v>
@@ -3139,7 +3142,7 @@
     </row>
     <row r="21">
       <c r="F21" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>74</v>
@@ -3147,7 +3150,7 @@
     </row>
     <row r="22">
       <c r="F22" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>76</v>
@@ -3155,7 +3158,7 @@
     </row>
     <row r="23">
       <c r="F23" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>157</v>
@@ -3163,7 +3166,7 @@
     </row>
     <row r="24">
       <c r="F24" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>187</v>
@@ -3171,7 +3174,7 @@
     </row>
     <row r="25">
       <c r="F25" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>187</v>
@@ -3179,7 +3182,7 @@
     </row>
     <row r="26">
       <c r="F26" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>82</v>
@@ -3187,7 +3190,7 @@
     </row>
     <row r="27">
       <c r="F27" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>113</v>
@@ -3254,7 +3257,7 @@
         <v>189</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36">
@@ -3262,7 +3265,7 @@
         <v>28</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37">
@@ -3270,7 +3273,7 @@
         <v>85</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38">
@@ -3278,20 +3281,20 @@
         <v>86</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39">
       <c r="F39" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40">
       <c r="F40" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>88</v>
@@ -3302,7 +3305,7 @@
         <v>17</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42">
@@ -3310,7 +3313,7 @@
         <v>87</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43">
@@ -3318,15 +3321,15 @@
         <v>89</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44">
       <c r="F44" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45">
@@ -3334,7 +3337,7 @@
         <v>90</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46">
@@ -3374,7 +3377,7 @@
         <v>99</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51">
@@ -3406,12 +3409,12 @@
         <v>107</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55">
       <c r="F55" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="P55" s="1" t="s">
         <v>105</v>
@@ -3419,7 +3422,7 @@
     </row>
     <row r="56">
       <c r="F56" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P56" s="1" t="s">
         <v>106</v>
@@ -3427,7 +3430,7 @@
     </row>
     <row r="57">
       <c r="F57" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="P57" s="1" t="s">
         <v>107</v>
@@ -3435,7 +3438,7 @@
     </row>
     <row r="58">
       <c r="F58" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="P58" s="1" t="s">
         <v>180</v>
@@ -3443,10 +3446,10 @@
     </row>
     <row r="59">
       <c r="F59" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60">
@@ -3454,7 +3457,7 @@
         <v>159</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="61">
@@ -3462,15 +3465,15 @@
         <v>163</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62">
       <c r="F62" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63">
@@ -3478,7 +3481,7 @@
         <v>62</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64">
@@ -3486,7 +3489,7 @@
         <v>155</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65">
@@ -3494,7 +3497,7 @@
         <v>41</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66">
@@ -3518,7 +3521,7 @@
         <v>68</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69">
@@ -3534,7 +3537,7 @@
         <v>136</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71">
@@ -3550,7 +3553,7 @@
         <v>38</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="73">
@@ -3558,7 +3561,7 @@
         <v>173</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74">
@@ -3566,7 +3569,7 @@
         <v>174</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="75">

</xml_diff>

<commit_message>
info for new patient
</commit_message>
<xml_diff>
--- a/clinical_info/Stim info.xlsx
+++ b/clinical_info/Stim info.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinconrad/Desktop/research/cceps/CCEPS/clinical_info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE2C8B4-B823-614A-B9DD-347EC2919917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Pt1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Pt2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Pt3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Pt4" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Pt5" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Pt6" sheetId="6" r:id="rId9"/>
+    <sheet name="Pt1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pt2" sheetId="2" r:id="rId2"/>
+    <sheet name="Pt3" sheetId="3" r:id="rId3"/>
+    <sheet name="Pt4" sheetId="4" r:id="rId4"/>
+    <sheet name="Pt5" sheetId="5" r:id="rId5"/>
+    <sheet name="Pt6" sheetId="6" r:id="rId6"/>
+    <sheet name="Pt7" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="329">
   <si>
     <t>Ieeg name</t>
   </si>
@@ -805,82 +815,269 @@
   </si>
   <si>
     <t>RH12</t>
+  </si>
+  <si>
+    <t>HUP218_CCEP</t>
+  </si>
+  <si>
+    <t>RA2</t>
+  </si>
+  <si>
+    <t>RA6</t>
+  </si>
+  <si>
+    <t>RA8</t>
+  </si>
+  <si>
+    <t>RB2</t>
+  </si>
+  <si>
+    <t>RC2</t>
+  </si>
+  <si>
+    <t>RC8</t>
+  </si>
+  <si>
+    <t>RD2</t>
+  </si>
+  <si>
+    <t>RD6</t>
+  </si>
+  <si>
+    <t>RE2</t>
+  </si>
+  <si>
+    <t>RE4</t>
+  </si>
+  <si>
+    <t>RG2</t>
+  </si>
+  <si>
+    <t>RG4</t>
+  </si>
+  <si>
+    <t>RG5</t>
+  </si>
+  <si>
+    <t>RG6</t>
+  </si>
+  <si>
+    <t>RG7</t>
+  </si>
+  <si>
+    <t>RI2</t>
+  </si>
+  <si>
+    <t>RI3</t>
+  </si>
+  <si>
+    <t>RI4</t>
+  </si>
+  <si>
+    <t>RK2</t>
+  </si>
+  <si>
+    <t>RK3</t>
+  </si>
+  <si>
+    <t>RK4</t>
+  </si>
+  <si>
+    <t>RL1</t>
+  </si>
+  <si>
+    <t>RL3</t>
+  </si>
+  <si>
+    <t>RL7</t>
+  </si>
+  <si>
+    <t>RL9</t>
+  </si>
+  <si>
+    <t>RM1</t>
+  </si>
+  <si>
+    <t>RM2</t>
+  </si>
+  <si>
+    <t>RM3</t>
+  </si>
+  <si>
+    <t>RM4</t>
+  </si>
+  <si>
+    <t>RM5</t>
+  </si>
+  <si>
+    <t>RM6</t>
+  </si>
+  <si>
+    <t>RM7</t>
+  </si>
+  <si>
+    <t>RN1</t>
+  </si>
+  <si>
+    <t>RN2</t>
+  </si>
+  <si>
+    <t>RN3</t>
+  </si>
+  <si>
+    <t>RN4</t>
+  </si>
+  <si>
+    <t>RN7</t>
+  </si>
+  <si>
+    <t>RP1</t>
+  </si>
+  <si>
+    <t>RP2</t>
+  </si>
+  <si>
+    <t>RP3</t>
+  </si>
+  <si>
+    <t>RR1</t>
+  </si>
+  <si>
+    <t>RR2</t>
+  </si>
+  <si>
+    <t>RR4</t>
+  </si>
+  <si>
+    <t>RR5</t>
+  </si>
+  <si>
+    <t>RR6</t>
+  </si>
+  <si>
+    <t>RR7</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>right mid cingulate</t>
+  </si>
+  <si>
+    <t>right superior frontal gyrus</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>right basal temporal</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>right orbitofrontal/PET</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>right anterior temporal revision</t>
+  </si>
+  <si>
+    <t>right orbitofrontal revision</t>
+  </si>
+  <si>
+    <t>right mesial frontal revision</t>
+  </si>
+  <si>
+    <t>right frontal pole revision</t>
+  </si>
+  <si>
+    <t>right anterior insula revision</t>
+  </si>
+  <si>
+    <t>mesial temporal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1070,20 +1267,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1133,12 +1333,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>12946.5</v>
@@ -1166,7 +1366,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1183,7 +1383,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
@@ -1194,7 +1394,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1205,27 +1405,28 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1275,12 +1476,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>18893.11</v>
@@ -1308,12 +1509,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="1">
-        <v>659035.32</v>
+        <v>659035.31999999995</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>43</v>
@@ -1328,7 +1529,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1342,7 +1543,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1356,7 +1557,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F6" s="1" t="s">
         <v>55</v>
       </c>
@@ -1370,7 +1571,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="1" t="s">
         <v>59</v>
       </c>
@@ -1384,7 +1585,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="1" t="s">
         <v>62</v>
       </c>
@@ -1398,7 +1599,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="1" t="s">
         <v>65</v>
       </c>
@@ -1409,7 +1610,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="1" t="s">
         <v>68</v>
       </c>
@@ -1420,7 +1621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="1" t="s">
         <v>70</v>
       </c>
@@ -1431,217 +1632,218 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F14" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F18" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F19" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F20" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F21" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F22" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F23" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F24" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F25" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F26" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F27" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F28" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F29" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F30" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F31" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F32" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F33" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F34" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F35" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F36" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F37" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F38" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F39" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F40" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F41" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F42" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F43" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F44" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F45" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F46" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F47" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="6:6" ht="13" x14ac:dyDescent="0.15">
       <c r="F48" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="6:6" ht="13" x14ac:dyDescent="0.15">
       <c r="F49" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="6:6" ht="13" x14ac:dyDescent="0.15">
       <c r="F50" s="1" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1691,12 +1893,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>7086.47</v>
@@ -1724,7 +1926,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F3" s="1" t="s">
         <v>79</v>
       </c>
@@ -1741,7 +1943,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F4" s="1" t="s">
         <v>81</v>
       </c>
@@ -1755,7 +1957,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F5" s="1" t="s">
         <v>113</v>
       </c>
@@ -1766,7 +1968,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F6" s="1" t="s">
         <v>110</v>
       </c>
@@ -1777,7 +1979,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="1" t="s">
         <v>76</v>
       </c>
@@ -1788,7 +1990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="1" t="s">
         <v>98</v>
       </c>
@@ -1799,7 +2001,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="1" t="s">
         <v>100</v>
       </c>
@@ -1810,7 +2012,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="1" t="s">
         <v>102</v>
       </c>
@@ -1821,7 +2023,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="1" t="s">
         <v>104</v>
       </c>
@@ -1832,7 +2034,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="1" t="s">
         <v>118</v>
       </c>
@@ -1843,7 +2045,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="1" t="s">
         <v>121</v>
       </c>
@@ -1854,7 +2056,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1865,7 +2067,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1876,7 +2078,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1887,7 +2089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F17" s="1" t="s">
         <v>128</v>
       </c>
@@ -1898,7 +2100,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F18" s="1" t="s">
         <v>70</v>
       </c>
@@ -1909,7 +2111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F19" s="1" t="s">
         <v>131</v>
       </c>
@@ -1920,122 +2122,123 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F20" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F21" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F22" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F23" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F24" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F25" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F26" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F27" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F28" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F29" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F31" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="6:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F32" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F33" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F34" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F35" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F36" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F37" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F38" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F39" s="1" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P70"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2085,12 +2288,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B2" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>13215.01</v>
@@ -2127,7 +2330,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>154</v>
       </c>
@@ -2156,7 +2359,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F4" s="1" t="s">
         <v>74</v>
       </c>
@@ -2176,7 +2379,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F5" s="1" t="s">
         <v>75</v>
       </c>
@@ -2193,7 +2396,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F6" s="1" t="s">
         <v>156</v>
       </c>
@@ -2210,7 +2413,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="1" t="s">
         <v>157</v>
       </c>
@@ -2227,7 +2430,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="1" t="s">
         <v>159</v>
       </c>
@@ -2241,7 +2444,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="1" t="s">
         <v>161</v>
       </c>
@@ -2255,7 +2458,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="1" t="s">
         <v>163</v>
       </c>
@@ -2269,7 +2472,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="1" t="s">
         <v>55</v>
       </c>
@@ -2283,7 +2486,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="1" t="s">
         <v>59</v>
       </c>
@@ -2297,7 +2500,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="1" t="s">
         <v>128</v>
       </c>
@@ -2311,7 +2514,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F14" s="1" t="s">
         <v>54</v>
       </c>
@@ -2325,7 +2528,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F15" s="1" t="s">
         <v>70</v>
       </c>
@@ -2333,7 +2536,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="1" t="s">
         <v>38</v>
       </c>
@@ -2341,7 +2544,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F17" s="1" t="s">
         <v>173</v>
       </c>
@@ -2349,7 +2552,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F18" s="1" t="s">
         <v>175</v>
       </c>
@@ -2357,7 +2560,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F19" s="1" t="s">
         <v>177</v>
       </c>
@@ -2365,7 +2568,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F20" s="1" t="s">
         <v>62</v>
       </c>
@@ -2373,7 +2576,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F21" s="1" t="s">
         <v>155</v>
       </c>
@@ -2381,7 +2584,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F22" s="1" t="s">
         <v>41</v>
       </c>
@@ -2389,7 +2592,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F23" s="1" t="s">
         <v>136</v>
       </c>
@@ -2397,7 +2600,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F24" s="1" t="s">
         <v>111</v>
       </c>
@@ -2405,7 +2608,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F25" s="1" t="s">
         <v>180</v>
       </c>
@@ -2413,7 +2616,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F26" s="1" t="s">
         <v>107</v>
       </c>
@@ -2421,7 +2624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F27" s="1" t="s">
         <v>106</v>
       </c>
@@ -2429,7 +2632,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F28" s="1" t="s">
         <v>94</v>
       </c>
@@ -2437,7 +2640,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F29" s="1" t="s">
         <v>93</v>
       </c>
@@ -2445,7 +2648,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F30" s="1" t="s">
         <v>105</v>
       </c>
@@ -2453,7 +2656,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F31" s="1" t="s">
         <v>92</v>
       </c>
@@ -2461,7 +2664,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F32" s="1" t="s">
         <v>91</v>
       </c>
@@ -2469,7 +2672,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F33" s="1" t="s">
         <v>90</v>
       </c>
@@ -2477,207 +2680,208 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P34" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P35" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P36" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P37" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P38" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P39" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P40" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P41" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P42" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P43" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P44" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P45" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P46" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P47" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P48" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P49" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P50" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P51" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P52" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P53" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P54" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P55" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P56" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P57" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P58" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P59" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P60" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P61" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P62" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P63" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P64" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P65" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P66" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P67" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P68" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P69" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="16:16" ht="13" x14ac:dyDescent="0.15">
       <c r="P70" s="2" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2727,7 +2931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>195</v>
       </c>
@@ -2744,72 +2948,75 @@
         <v>170.95</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" s="1">
-        <v>1051.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E4" s="1">
-        <v>2168.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" s="1">
-        <v>3099.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>3099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E6" s="1">
-        <v>4031.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E7" s="1">
-        <v>4978.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>4978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E8" s="1">
-        <v>6110.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>6110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E9" s="1">
-        <v>7027.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>7027</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E10" s="1">
-        <v>8031.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>8031</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E11" s="1">
-        <v>8806.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>8806</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E12" s="1">
-        <v>9347.8</v>
+        <v>9347.7999999999993</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2859,12 +3066,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>198</v>
       </c>
       <c r="B2" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>25875.11</v>
@@ -2894,7 +3101,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>204</v>
       </c>
@@ -2914,7 +3121,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F4" s="1" t="s">
         <v>206</v>
       </c>
@@ -2928,7 +3135,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F5" s="1" t="s">
         <v>207</v>
       </c>
@@ -2942,7 +3149,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2956,7 +3163,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="1" t="s">
         <v>209</v>
       </c>
@@ -2970,7 +3177,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="1" t="s">
         <v>210</v>
       </c>
@@ -2984,7 +3191,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="1" t="s">
         <v>211</v>
       </c>
@@ -2998,7 +3205,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="1" t="s">
         <v>141</v>
       </c>
@@ -3012,7 +3219,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="1" t="s">
         <v>213</v>
       </c>
@@ -3026,7 +3233,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="1" t="s">
         <v>215</v>
       </c>
@@ -3040,7 +3247,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="1" t="s">
         <v>137</v>
       </c>
@@ -3054,7 +3261,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F14" s="1" t="s">
         <v>138</v>
       </c>
@@ -3068,7 +3275,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F15" s="1" t="s">
         <v>139</v>
       </c>
@@ -3082,7 +3289,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="1" t="s">
         <v>220</v>
       </c>
@@ -3096,7 +3303,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F17" s="1" t="s">
         <v>222</v>
       </c>
@@ -3110,7 +3317,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F18" s="1" t="s">
         <v>224</v>
       </c>
@@ -3124,7 +3331,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F19" s="1" t="s">
         <v>226</v>
       </c>
@@ -3132,7 +3339,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F20" s="1" t="s">
         <v>227</v>
       </c>
@@ -3140,7 +3347,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F21" s="1" t="s">
         <v>228</v>
       </c>
@@ -3148,7 +3355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F22" s="1" t="s">
         <v>229</v>
       </c>
@@ -3156,7 +3363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F23" s="1" t="s">
         <v>230</v>
       </c>
@@ -3164,7 +3371,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F24" s="1" t="s">
         <v>231</v>
       </c>
@@ -3172,7 +3379,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F25" s="1" t="s">
         <v>232</v>
       </c>
@@ -3180,7 +3387,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F26" s="1" t="s">
         <v>233</v>
       </c>
@@ -3188,7 +3395,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F27" s="1" t="s">
         <v>234</v>
       </c>
@@ -3196,7 +3403,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F28" s="1" t="s">
         <v>73</v>
       </c>
@@ -3204,7 +3411,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F29" s="1" t="s">
         <v>75</v>
       </c>
@@ -3212,7 +3419,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F30" s="1" t="s">
         <v>77</v>
       </c>
@@ -3220,7 +3427,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F31" s="1" t="s">
         <v>186</v>
       </c>
@@ -3228,7 +3435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F32" s="1" t="s">
         <v>78</v>
       </c>
@@ -3236,7 +3443,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F33" s="1" t="s">
         <v>80</v>
       </c>
@@ -3244,7 +3451,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F34" s="1" t="s">
         <v>82</v>
       </c>
@@ -3252,7 +3459,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F35" s="1" t="s">
         <v>189</v>
       </c>
@@ -3260,7 +3467,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F36" s="1" t="s">
         <v>28</v>
       </c>
@@ -3268,7 +3475,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F37" s="1" t="s">
         <v>85</v>
       </c>
@@ -3276,7 +3483,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F38" s="1" t="s">
         <v>86</v>
       </c>
@@ -3284,7 +3491,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F39" s="1" t="s">
         <v>236</v>
       </c>
@@ -3292,7 +3499,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F40" s="1" t="s">
         <v>237</v>
       </c>
@@ -3300,7 +3507,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F41" s="1" t="s">
         <v>17</v>
       </c>
@@ -3308,7 +3515,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F42" s="1" t="s">
         <v>87</v>
       </c>
@@ -3316,7 +3523,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F43" s="1" t="s">
         <v>89</v>
       </c>
@@ -3324,7 +3531,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F44" s="1" t="s">
         <v>241</v>
       </c>
@@ -3332,7 +3539,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F45" s="1" t="s">
         <v>90</v>
       </c>
@@ -3340,7 +3547,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F46" s="1" t="s">
         <v>92</v>
       </c>
@@ -3348,7 +3555,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="6:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F47" s="1" t="s">
         <v>94</v>
       </c>
@@ -3356,7 +3563,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F48" s="1" t="s">
         <v>96</v>
       </c>
@@ -3364,7 +3571,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F49" s="1" t="s">
         <v>98</v>
       </c>
@@ -3372,7 +3579,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F50" s="1" t="s">
         <v>99</v>
       </c>
@@ -3380,7 +3587,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F51" s="1" t="s">
         <v>100</v>
       </c>
@@ -3388,7 +3595,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F52" s="1" t="s">
         <v>101</v>
       </c>
@@ -3396,7 +3603,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F53" s="1" t="s">
         <v>105</v>
       </c>
@@ -3404,7 +3611,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F54" s="1" t="s">
         <v>107</v>
       </c>
@@ -3412,7 +3619,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F55" s="1" t="s">
         <v>247</v>
       </c>
@@ -3420,7 +3627,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F56" s="1" t="s">
         <v>248</v>
       </c>
@@ -3428,7 +3635,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F57" s="1" t="s">
         <v>249</v>
       </c>
@@ -3436,7 +3643,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F58" s="1" t="s">
         <v>250</v>
       </c>
@@ -3444,7 +3651,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F59" s="1" t="s">
         <v>251</v>
       </c>
@@ -3452,7 +3659,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F60" s="1" t="s">
         <v>159</v>
       </c>
@@ -3460,7 +3667,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F61" s="1" t="s">
         <v>163</v>
       </c>
@@ -3468,7 +3675,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F62" s="1" t="s">
         <v>255</v>
       </c>
@@ -3476,7 +3683,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F63" s="1" t="s">
         <v>62</v>
       </c>
@@ -3484,7 +3691,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F64" s="1" t="s">
         <v>155</v>
       </c>
@@ -3492,7 +3699,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F65" s="1" t="s">
         <v>41</v>
       </c>
@@ -3500,7 +3707,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F66" s="1" t="s">
         <v>46</v>
       </c>
@@ -3508,7 +3715,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F67" s="1" t="s">
         <v>65</v>
       </c>
@@ -3516,7 +3723,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F68" s="1" t="s">
         <v>68</v>
       </c>
@@ -3524,7 +3731,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F69" s="1" t="s">
         <v>135</v>
       </c>
@@ -3532,7 +3739,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F70" s="1" t="s">
         <v>136</v>
       </c>
@@ -3540,7 +3747,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F71" s="1" t="s">
         <v>70</v>
       </c>
@@ -3548,7 +3755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F72" s="1" t="s">
         <v>38</v>
       </c>
@@ -3556,7 +3763,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F73" s="1" t="s">
         <v>173</v>
       </c>
@@ -3564,7 +3771,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F74" s="1" t="s">
         <v>174</v>
       </c>
@@ -3572,37 +3779,546 @@
         <v>262</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F75" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F76" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F77" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F78" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F79" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="6:16" ht="13" x14ac:dyDescent="0.15">
       <c r="F80" s="1" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1371A68E-4402-9949-A7EB-39EF0B9EBBFF}">
+  <dimension ref="A1:P64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I2" t="s">
+        <v>310</v>
+      </c>
+      <c r="J2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K2" t="s">
+        <v>310</v>
+      </c>
+      <c r="M2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F4" t="s">
+        <v>205</v>
+      </c>
+      <c r="M4" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F5" t="s">
+        <v>265</v>
+      </c>
+      <c r="M5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F6" t="s">
+        <v>207</v>
+      </c>
+      <c r="M6" t="s">
+        <v>126</v>
+      </c>
+      <c r="N6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F7" t="s">
+        <v>266</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>130</v>
+      </c>
+      <c r="N9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F10" t="s">
+        <v>267</v>
+      </c>
+      <c r="M10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F11" t="s">
+        <v>209</v>
+      </c>
+      <c r="M11" t="s">
+        <v>313</v>
+      </c>
+      <c r="N11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M12" t="s">
+        <v>314</v>
+      </c>
+      <c r="N12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F13" t="s">
+        <v>268</v>
+      </c>
+      <c r="M13" t="s">
+        <v>315</v>
+      </c>
+      <c r="N13" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F14" t="s">
+        <v>269</v>
+      </c>
+      <c r="M14" t="s">
+        <v>317</v>
+      </c>
+      <c r="N14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F15" t="s">
+        <v>211</v>
+      </c>
+      <c r="M15" t="s">
+        <v>318</v>
+      </c>
+      <c r="N15" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="F16" t="s">
+        <v>270</v>
+      </c>
+      <c r="M16" t="s">
+        <v>322</v>
+      </c>
+      <c r="N16" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F17" t="s">
+        <v>141</v>
+      </c>
+      <c r="M17" t="s">
+        <v>319</v>
+      </c>
+      <c r="N17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F18" t="s">
+        <v>142</v>
+      </c>
+      <c r="M18" t="s">
+        <v>320</v>
+      </c>
+      <c r="N18" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F22" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F29" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F30" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.15">
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F33" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F34" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F35" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F37" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F38" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F40" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F41" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F42" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F45" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F47" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F48" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F49" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F50" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F51" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F52" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F53" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F54" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F55" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F56" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F57" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F58" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F59" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F60" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F61" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F62" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F63" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F64" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>